<commit_message>
2024/4/9 report and other files
</commit_message>
<xml_diff>
--- a/Others/gantt.xlsx
+++ b/Others/gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Recommendation system\202018010410_project_recommendation-system\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BDD352-F78A-40DC-BEFA-5B5D955E4BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2A6F67-2202-4D84-AB7D-845BDC128BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -31,9 +31,6 @@
     <t xml:space="preserve">End Date </t>
   </si>
   <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Investigation on the Existing Food Delivery Platform</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -42,35 +39,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Determine a feasible recommender system model</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Research on Collaborative Filtering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Project proposal</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Requirement analysis</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>System design</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Implementation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Implement the recommend function</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test and evaluate the recommend function</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -82,7 +51,55 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>System testing</t>
+    <t>Write Project proposal</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Research on recommendation system</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duration</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Research on CF and Content-based recommendation</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function requirements analysis</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>System design (divided into several modules)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database design</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Implementation </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Progress report</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recommend function design</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Develop recommend function</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>System testing &amp; performance analysis</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test and evaluate website function</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -178,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -189,6 +206,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -261,9 +281,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>Investigation on the Existing Food Delivery Platform</c:v>
                 </c:pt>
@@ -271,36 +291,48 @@
                   <c:v>Comparison between food delivery platform</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Research on Collaborative Filtering</c:v>
+                  <c:v>Research on recommendation system</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Determine a feasible recommender system model</c:v>
+                  <c:v>Write Project proposal</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Research on CF and Content-based recommendation</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Project proposal</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Requirement analysis</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>System design</c:v>
+                  <c:v>Function requirements analysis</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Implementation</c:v>
+                  <c:v>System design (divided into several modules)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Implement the recommend function</c:v>
+                  <c:v>Database design</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Test and evaluate the recommend function</c:v>
+                  <c:v>Web Implementation </c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>System testing</c:v>
+                  <c:v>Progress report</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Recommend function design</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Develop recommend function</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Test and evaluate website function</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>System testing &amp; performance analysis</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Final report</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>Create Poster</c:v>
                 </c:pt>
               </c:strCache>
@@ -308,10 +340,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>45215</c:v>
                 </c:pt>
@@ -319,36 +351,48 @@
                   <c:v>45219</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>45223</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45224</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45228</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>45221</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>45223</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45221</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45233</c:v>
-                </c:pt>
                 <c:pt idx="6">
+                  <c:v>45231</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>45244</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>45250</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>45261</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>45301</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>45270</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45293</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45302</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>45332</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>45333</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>45331</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>45367</c:v>
                 </c:pt>
               </c:numCache>
@@ -519,9 +563,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>Investigation on the Existing Food Delivery Platform</c:v>
                 </c:pt>
@@ -529,36 +573,48 @@
                   <c:v>Comparison between food delivery platform</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Research on Collaborative Filtering</c:v>
+                  <c:v>Research on recommendation system</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Determine a feasible recommender system model</c:v>
+                  <c:v>Write Project proposal</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Research on CF and Content-based recommendation</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Project proposal</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Requirement analysis</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>System design</c:v>
+                  <c:v>Function requirements analysis</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Implementation</c:v>
+                  <c:v>System design (divided into several modules)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Implement the recommend function</c:v>
+                  <c:v>Database design</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Test and evaluate the recommend function</c:v>
+                  <c:v>Web Implementation </c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>System testing</c:v>
+                  <c:v>Progress report</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Recommend function design</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Develop recommend function</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Test and evaluate website function</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>System testing &amp; performance analysis</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Final report</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>Create Poster</c:v>
                 </c:pt>
               </c:strCache>
@@ -566,47 +622,59 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$14</c:f>
+              <c:f>Sheet1!$D$2:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>62</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
@@ -1335,15 +1403,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>102130</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:colOff>102131</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>17927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>843962</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>43543</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>900545</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1629,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1654,12 +1722,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>45215</v>
@@ -1668,239 +1736,307 @@
         <v>45225</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D3" si="0">C2-B2</f>
+        <f t="shared" ref="D2" si="0">C2-B2</f>
         <v>10</v>
       </c>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
+      <c r="A3" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>45219</v>
       </c>
       <c r="C3" s="3">
-        <v>45230</v>
+        <v>45227</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>C3-B3</f>
+        <v>8</v>
       </c>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
+      <c r="A4" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>45221</v>
+        <v>45223</v>
       </c>
       <c r="C4" s="4">
-        <v>45231</v>
+        <v>45228</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D14" si="1">C4-B4</f>
-        <v>10</v>
+        <f t="shared" ref="D4:D18" si="1">C4-B4</f>
+        <v>5</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
+      <c r="A5" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="B5" s="3">
-        <v>45223</v>
-      </c>
-      <c r="C5" s="3">
+        <v>45224</v>
+      </c>
+      <c r="C5" s="4">
         <v>45233</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45217</v>
-      </c>
-      <c r="G5" s="8">
-        <v>45385</v>
+        <f>C5-B5</f>
+        <v>9</v>
       </c>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
+      <c r="A6" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>45221</v>
+        <v>45228</v>
       </c>
       <c r="C6" s="3">
-        <v>45233</v>
+        <v>45240</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ref="D6" si="2">C6-B6</f>
+        <f t="shared" si="1"/>
         <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45217</v>
+      </c>
+      <c r="G6" s="8">
+        <v>45385</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
+      <c r="A7" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="B7" s="3">
+        <v>45221</v>
+      </c>
+      <c r="C7" s="3">
         <v>45233</v>
       </c>
-      <c r="C7" s="3">
-        <v>45248</v>
-      </c>
       <c r="D7" s="2">
-        <f>C7-B7</f>
-        <v>15</v>
+        <f t="shared" ref="D7" si="2">C7-B7</f>
+        <v>12</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
+      <c r="A8" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>45244</v>
+        <v>45231</v>
       </c>
       <c r="C8" s="3">
-        <v>45260</v>
-      </c>
-      <c r="D8" s="5">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <v>45248</v>
+      </c>
+      <c r="D8" s="2">
+        <f>C8-B8</f>
+        <v>17</v>
       </c>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
+      <c r="A9" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>45261</v>
-      </c>
-      <c r="C9" s="4">
-        <v>45323</v>
-      </c>
-      <c r="D9" s="2">
+        <v>45244</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45260</v>
+      </c>
+      <c r="D9" s="5">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
+      <c r="A10" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>45301</v>
+        <v>45250</v>
       </c>
       <c r="C10" s="3">
-        <v>45331</v>
-      </c>
-      <c r="D10" s="2">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <v>45256</v>
+      </c>
+      <c r="D10" s="5">
+        <f>C10-B10</f>
+        <v>6</v>
       </c>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
+      <c r="A11" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="3">
+        <v>45261</v>
+      </c>
+      <c r="C11" s="4">
         <v>45332</v>
-      </c>
-      <c r="C11" s="6">
-        <v>45342</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3">
-        <v>45333</v>
-      </c>
-      <c r="C12" s="6">
-        <v>45343</v>
+        <v>45270</v>
+      </c>
+      <c r="C12" s="4">
+        <v>45287</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
+      <c r="A13" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="B13" s="3">
-        <v>45331</v>
-      </c>
-      <c r="C13" s="6">
-        <v>45366</v>
+        <v>45293</v>
+      </c>
+      <c r="C13" s="4">
+        <v>45301</v>
       </c>
       <c r="D13" s="2">
-        <f>C13-B13</f>
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="1:16" ht="16.2" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
+    <row r="14" spans="1:16">
+      <c r="A14" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="B14" s="3">
-        <v>45367</v>
-      </c>
-      <c r="C14" s="6">
-        <v>45397</v>
+        <v>45302</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45352</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="1:16" ht="16.2" customHeight="1">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="9"/>
+    <row r="15" spans="1:16">
+      <c r="A15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45332</v>
+      </c>
+      <c r="C15" s="6">
+        <v>45342</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="16.2" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="9"/>
+    <row r="16" spans="1:16">
+      <c r="A16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45333</v>
+      </c>
+      <c r="C16" s="6">
+        <v>45343</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45331</v>
+      </c>
+      <c r="C17" s="6">
+        <v>45366</v>
+      </c>
+      <c r="D17" s="2">
+        <f>C17-B17</f>
+        <v>35</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="1:16" ht="16.2" customHeight="1">
+      <c r="A18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3">
+        <v>45367</v>
+      </c>
+      <c r="C18" s="6">
+        <v>45397</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="1:16" ht="16.2" customHeight="1">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="9"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:16" ht="16.2" customHeight="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="9"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>